<commit_message>
Atualização automática de AUGUSTO_PESTANA.xlsx
</commit_message>
<xml_diff>
--- a/AUGUSTO_PESTANA.xlsx
+++ b/AUGUSTO_PESTANA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D11F306-9EBE-4621-BFA2-7DEDEF52CBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC55A4B8-5766-4767-988F-6785FE76F3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1135,7 +1122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1195,36 +1182,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1258,14 +1221,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1279,7 +1238,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1322,7 +1280,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{968B1FF3-6AA1-4F21-A3E6-4EA9C33B6128}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{CD5EE669-6FF1-44A9-A7FB-7DEB6C1B888E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1352,10 +1310,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26330613-B5DE-4A73-9AE2-482678BB34D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24D2C54-3B81-44AB-B942-257DD93A2A4F}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1393,7 +1351,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13B0915D-FF2C-4F1F-A064-4EFB910574E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF9A725-E871-40B9-86D8-EC03769E4B3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1456,7 +1414,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B8A603A-2D68-42CB-94B1-1C38F6A65D2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB7E0842-FA30-42D0-A698-B337A4C9E01E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1475,7 +1433,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AA9AD65-85D0-39D4-3348-762BBCC16CBC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4C9EBB6-86D6-F384-0312-EC86D55CA9F5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1524,7 +1482,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE105DC2-6C70-328D-B4DF-B69AAD45D9BA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E73CA9-082A-BD6E-B7D2-C0D25531C2BF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1543,7 +1501,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A93F76DA-1CC8-3796-49B8-CAA7B8927A3F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70F82316-6493-AA5F-E659-92622327F7C8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1574,7 +1532,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F8DDFE2-5494-FD29-C20C-773A1DBE155A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FD93D10-9980-5663-9603-3321E02DF649}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,7 +1563,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4F447B1-1A98-6850-1F22-3A158D384060}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20A011DC-31BC-78D5-E231-EB0234B1FB14}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1648,7 +1606,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01400FF3-41ED-44C3-9B88-AE34B0D8F90D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426C768F-8BA1-42F0-9A3E-D10318251210}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1686,7 +1644,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74E00D4B-4407-4B6A-B9CD-8D59C91907CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A62ABE-C765-4386-B467-ECD3879985E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1729,7 +1687,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E01FFB9A-E5CD-4062-9E70-BF744D5AAEAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E81337-E896-4ABA-816B-847A96F25107}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2042,7 +2000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE1D3B1-8D6C-418D-88E7-C0D5909D9F2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F43AD7-54AE-4B84-83B0-51EAFF34D8F2}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2054,98 +2012,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="39"/>
-    <col min="6" max="6" width="2" style="39" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="39" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="39"/>
+    <col min="1" max="5" width="12.5703125" style="36"/>
+    <col min="6" max="6" width="2" style="36" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="38"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="38"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="38"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="38"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="38"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="38"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="38"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="38"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="38"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="38"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="38"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="38"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="38"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="38"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="38"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="38"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="38"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="38"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="38"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="38"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="38"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="38"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="38"/>
+      <c r="F23" s="35"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="38"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="38"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="38"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="38"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="38"/>
+      <c r="F28" s="35"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="38"/>
+      <c r="F29" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5292,19 +5250,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5327,35 +5285,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>262</v>
       </c>
     </row>
@@ -5373,1135 +5331,1135 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="14">
         <v>720420500</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="20">
         <v>36</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="20">
         <v>3.6</v>
       </c>
-      <c r="F2" s="22">
-        <v>6</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="14">
+        <v>6</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="14">
         <v>720420600</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="20">
         <v>36</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="20">
         <v>3.6</v>
       </c>
-      <c r="F3" s="22">
-        <v>6</v>
-      </c>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="14">
+        <v>6</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="14">
         <v>720420700</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <v>36</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="20">
         <v>3.6</v>
       </c>
-      <c r="F4" s="22">
-        <v>6</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="14">
+        <v>6</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="14">
         <v>720421000</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>36</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>3.6</v>
       </c>
-      <c r="F5" s="22">
-        <v>6</v>
-      </c>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="14">
+        <v>6</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="14">
         <v>720424200</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>36</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>3.6</v>
       </c>
-      <c r="F6" s="22">
-        <v>6</v>
-      </c>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="14">
+        <v>6</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="14">
         <v>720431300</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>36</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>3.6</v>
       </c>
-      <c r="F7" s="22">
-        <v>6</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="14">
+        <v>6</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="14">
         <v>720435500</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>36</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>3.6</v>
       </c>
-      <c r="F8" s="22">
-        <v>6</v>
-      </c>
-      <c r="G8" s="22" t="s">
+      <c r="F8" s="14">
+        <v>6</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="14">
         <v>720436100</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>36</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <v>3.6</v>
       </c>
-      <c r="F9" s="22">
-        <v>6</v>
-      </c>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="14">
+        <v>6</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="14">
         <v>720437500</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>36</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>3.6</v>
       </c>
-      <c r="F10" s="22">
-        <v>6</v>
-      </c>
-      <c r="G10" s="22" t="s">
+      <c r="F10" s="14">
+        <v>6</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="14">
         <v>720438500</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <v>36</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>3.6</v>
       </c>
-      <c r="F11" s="22">
-        <v>6</v>
-      </c>
-      <c r="G11" s="22" t="s">
+      <c r="F11" s="14">
+        <v>6</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="14">
         <v>720439900</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>36</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>3.6</v>
       </c>
-      <c r="F12" s="22">
-        <v>6</v>
-      </c>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="14">
+        <v>6</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="14">
         <v>720442800</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="20">
         <v>36</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <v>3.6</v>
       </c>
-      <c r="F13" s="22">
-        <v>6</v>
-      </c>
-      <c r="G13" s="22" t="s">
+      <c r="F13" s="14">
+        <v>6</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="14">
         <v>730515500</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="20">
         <v>15.89</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="20">
         <v>1.59</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="14">
         <v>5</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="14">
         <v>730515600</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="20">
         <v>15.89</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="20">
         <v>1.59</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="14">
         <v>5</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="14">
         <v>730515700</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="20">
         <v>15.89</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="20">
         <v>1.59</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="14">
         <v>5</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="14">
         <v>730515800</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="20">
         <v>15.89</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="20">
         <v>1.59</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="14">
         <v>5</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="14">
         <v>730516000</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="20">
         <v>15.89</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="20">
         <v>1.59</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="14">
         <v>5</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="14">
         <v>9990050500</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="20">
         <v>60</v>
       </c>
-      <c r="E19" s="23">
-        <v>6</v>
-      </c>
-      <c r="F19" s="22">
+      <c r="E19" s="20">
+        <v>6</v>
+      </c>
+      <c r="F19" s="14">
         <v>25</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="21">
         <v>11603</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="14">
         <v>9990050600</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="20">
         <v>60</v>
       </c>
-      <c r="E20" s="23">
-        <v>6</v>
-      </c>
-      <c r="F20" s="22">
+      <c r="E20" s="20">
+        <v>6</v>
+      </c>
+      <c r="F20" s="14">
         <v>25</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="21">
         <v>11603</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="14">
         <v>9990050700</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="20">
         <v>60</v>
       </c>
-      <c r="E21" s="23">
-        <v>6</v>
-      </c>
-      <c r="F21" s="22">
+      <c r="E21" s="20">
+        <v>6</v>
+      </c>
+      <c r="F21" s="14">
         <v>25</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="14">
         <v>121310500</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="20">
         <v>52</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="20">
         <v>5.2</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="14">
         <v>0</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="21">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="14">
         <v>49642</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="20">
         <v>142.4</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="20">
         <v>14.24</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="14">
         <v>0</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="21">
         <v>11096</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="14">
         <v>119782</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="20">
         <v>169</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="20">
         <v>16.899999999999999</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="14">
         <v>12</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="14">
         <v>130603</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="20">
         <v>800</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="20">
         <v>80</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="14">
         <v>3.4</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I25" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="K25" s="24">
+      <c r="K25" s="21">
         <v>12454</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="14">
         <v>124283</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="20">
         <v>588.48</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="20">
         <v>58.85</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="14">
         <v>35</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="I26" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K26" s="24">
+      <c r="K26" s="21">
         <v>516</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="14">
         <v>163978</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="20">
         <v>550</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="20">
         <v>55</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="14">
         <v>3</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="21">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="14">
         <v>176979</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="20">
         <v>2050</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="20">
         <v>205</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="14">
         <v>10</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K28" s="24">
+      <c r="K28" s="21">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="14">
         <v>288698</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="20">
         <v>3518.22</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="20">
         <v>351.82</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="14">
         <v>5</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="K29" s="24">
+      <c r="K29" s="21">
         <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="14">
         <v>347384</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="20">
         <v>2560</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="20">
         <v>256</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="14">
         <v>64</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H30" s="22" t="s">
+      <c r="H30" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I30" s="22" t="s">
+      <c r="I30" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J30" s="22" t="s">
+      <c r="J30" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="K30" s="24">
+      <c r="K30" s="21">
         <v>12454</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="14">
         <v>377481</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="20">
         <v>3120</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="20">
         <v>312</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="14">
         <v>15</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H31" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="K31" s="24">
+      <c r="K31" s="21">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="14">
         <v>538850</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="20">
         <v>2882.4</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="20">
         <v>2623.08</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="14">
         <v>17.3</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I32" s="22" t="s">
+      <c r="I32" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="J32" s="22" t="s">
+      <c r="J32" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="K32" s="24">
+      <c r="K32" s="21">
         <v>11097</v>
       </c>
     </row>
@@ -6526,101 +6484,102 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="22" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="25">
         <v>45717</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="26">
         <v>1717</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="27">
         <v>3121</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="27">
         <v>483</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>320</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="29" t="s">
         <v>320</v>
       </c>
     </row>
@@ -6645,31 +6604,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>322</v>
       </c>
-      <c r="E1" s="34">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="31">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="34">
         <v>5</v>
       </c>
-      <c r="F1" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>273</v>
-      </c>
-      <c r="B2" s="37">
-        <v>5</v>
-      </c>
-      <c r="C2" s="35">
+      <c r="C2" s="32">
         <v>3.3064409469646871E-4</v>
       </c>
     </row>

</xml_diff>